<commit_message>
got rpt sttus of dqa andd cqa
</commit_message>
<xml_diff>
--- a/C&DQA/FinishedReport/KELLY1/KELLY1Report.xlsx
+++ b/C&DQA/FinishedReport/KELLY1/KELLY1Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>Appendix I</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Total Molybdenum (Mo)</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>Total Zinc (Zn)</t>
@@ -348,7 +351,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -531,6 +534,10 @@
       <sz val="11"/>
       <vertAlign val="superscript"/>
     </font>
+    <font>
+      <name val="Franklin Gothic Book"/>
+      <b val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -552,7 +559,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="89">
+  <borders count="93">
     <border>
       <left/>
       <right/>
@@ -1300,6 +1307,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="medium"/>
@@ -1498,10 +1512,36 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium"/>
       <right/>
       <top/>
-      <bottom style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1518,11 +1558,18 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="268">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -2173,12 +2220,15 @@
     <xf applyAlignment="1" borderId="46" fillId="0" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="54" fillId="2" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="55" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="56" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf applyAlignment="1" borderId="56" fillId="2" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="57" fillId="2" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2186,56 +2236,98 @@
     <xf applyAlignment="1" borderId="58" fillId="2" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="67" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="63" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="64" fillId="2" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf borderId="68" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="64" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="65" fillId="2" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="66" fillId="2" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="66" fillId="2" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="67" fillId="2" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="69" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="70" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="71" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="71" fillId="2" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="72" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="71" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="72" fillId="2" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="73" fillId="2" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="75" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="72" fillId="2" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="73" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="74" fillId="2" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="76" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="18" fillId="0" fontId="28" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="23" fillId="0" fontId="28" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="77" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="30" fillId="0" fontId="28" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="54" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="77" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="78" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="56" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="78" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="79" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="79" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="80" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="81" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="82" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="83" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="38" fillId="2" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="41" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="84" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="30" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="85" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="41" fillId="0" fontId="28" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="86" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="62" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="90" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="53" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="18" fillId="2" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="91" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="87" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="53" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="88" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="92" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="88" fillId="2" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="89" fillId="2" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="28" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="22" fillId="0" fontId="28" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="31" fillId="0" fontId="28" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2273,7 +2365,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>8</col>
+      <col>7</col>
       <colOff>0</colOff>
       <row>1</row>
       <rowOff>0</rowOff>
@@ -2298,7 +2390,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>1</col>
+      <col>0</col>
       <colOff>0</colOff>
       <row>46</row>
       <rowOff>0</rowOff>
@@ -2323,7 +2415,7 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>8</col>
+      <col>7</col>
       <colOff>0</colOff>
       <row>46</row>
       <rowOff>0</rowOff>
@@ -2675,87 +2767,95 @@
     <col customWidth="1" max="16384" min="15" style="24" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9"/>
-    <row r="2" spans="1:9"/>
+    <row r="1" spans="1:9">
+      <c s="220" r="D1" t="n"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c s="220" r="D2" t="n"/>
+    </row>
     <row r="3" spans="1:9">
       <c s="200" r="A3" t="s">
         <v>0</v>
       </c>
+      <c s="220" r="D3" t="n"/>
     </row>
     <row r="4" spans="1:9">
       <c s="200" r="A4" t="s">
         <v>1</v>
       </c>
+      <c s="220" r="D4" t="n"/>
     </row>
     <row r="5" spans="1:9">
       <c s="201" r="A5" t="s">
         <v>2</v>
       </c>
+      <c s="220" r="D5" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="6" ht="17.25" spans="1:9">
       <c s="185" r="A6" t="s">
         <v>3</v>
       </c>
+      <c s="220" r="D6" t="n"/>
     </row>
     <row customHeight="1" r="7" ht="16.5" spans="1:9">
-      <c s="220" r="B7" t="s">
+      <c s="221" r="B7" t="s">
         <v>4</v>
       </c>
-      <c s="221" r="C7" t="n"/>
-      <c s="222" r="D7" t="s">
+      <c s="222" r="C7" t="n"/>
+      <c s="223" r="D7" t="s">
         <v>5</v>
       </c>
-      <c s="223" r="E7" t="s">
+      <c s="224" r="E7" t="s">
         <v>6</v>
       </c>
-      <c s="221" r="F7" t="n"/>
-      <c s="221" r="G7" t="n"/>
-      <c s="221" r="H7" t="n"/>
-      <c s="224" r="I7" t="s">
+      <c s="222" r="F7" t="n"/>
+      <c s="222" r="G7" t="n"/>
+      <c s="222" r="H7" t="n"/>
+      <c s="225" r="I7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c s="225" r="B8" t="n"/>
-      <c s="221" r="C8" t="n"/>
-      <c s="226" r="D8" t="n"/>
-      <c s="227" r="E8" t="s">
+      <c s="226" r="B8" t="n"/>
+      <c s="222" r="C8" t="n"/>
+      <c s="227" r="D8" t="n"/>
+      <c s="228" r="E8" t="s">
         <v>8</v>
       </c>
-      <c s="221" r="F8" t="n"/>
-      <c s="228" r="G8" t="s">
+      <c s="222" r="F8" t="n"/>
+      <c s="229" r="G8" t="s">
         <v>9</v>
       </c>
-      <c s="221" r="H8" t="n"/>
-      <c s="229" r="I8" t="s">
+      <c s="222" r="H8" t="n"/>
+      <c s="230" r="I8" t="s">
         <v>10</v>
       </c>
     </row>
     <row customHeight="1" r="9" ht="15.75" spans="1:9">
-      <c s="225" r="B9" t="n"/>
-      <c s="221" r="C9" t="n"/>
-      <c s="226" r="D9" t="n"/>
-      <c s="221" r="E9" t="n"/>
-      <c s="221" r="F9" t="n"/>
-      <c s="221" r="G9" t="n"/>
-      <c s="230" r="H9" t="n"/>
-      <c s="231" r="I9" t="n"/>
+      <c s="226" r="B9" t="n"/>
+      <c s="222" r="C9" t="n"/>
+      <c s="227" r="D9" t="n"/>
+      <c s="222" r="E9" t="n"/>
+      <c s="222" r="F9" t="n"/>
+      <c s="222" r="G9" t="n"/>
+      <c s="231" r="H9" t="n"/>
+      <c s="232" r="I9" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="10" ht="16.5" spans="1:9">
-      <c s="225" r="B10" t="n"/>
-      <c s="221" r="C10" t="n"/>
-      <c s="232" r="D10" t="s">
+      <c s="226" r="B10" t="n"/>
+      <c s="222" r="C10" t="n"/>
+      <c s="233" r="D10" t="s">
         <v>11</v>
       </c>
-      <c s="233" r="E10" t="s">
+      <c s="234" r="E10" t="s">
         <v>11</v>
       </c>
-      <c s="221" r="F10" t="n"/>
-      <c s="234" r="G10" t="s">
+      <c s="222" r="F10" t="n"/>
+      <c s="235" r="G10" t="s">
         <v>11</v>
       </c>
-      <c s="221" r="H10" t="n"/>
-      <c s="235" r="I10" t="s">
+      <c s="222" r="H10" t="n"/>
+      <c s="236" r="I10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2763,18 +2863,18 @@
       <c s="210" r="B11" t="s">
         <v>13</v>
       </c>
-      <c s="236" r="C11" t="n"/>
-      <c s="49" r="D11" t="s">
+      <c s="237" r="C11" t="n"/>
+      <c s="238" r="D11" t="s">
         <v>14</v>
       </c>
       <c s="212" r="E11" t="n">
         <v>13</v>
       </c>
-      <c s="236" r="F11" t="n"/>
+      <c s="237" r="F11" t="n"/>
       <c s="212" r="G11" t="n">
         <v>75</v>
       </c>
-      <c s="236" r="H11" t="n"/>
+      <c s="237" r="H11" t="n"/>
       <c s="13" r="I11" t="n">
         <v>15</v>
       </c>
@@ -2783,18 +2883,18 @@
       <c s="203" r="B12" t="s">
         <v>15</v>
       </c>
-      <c s="236" r="C12" t="n"/>
-      <c s="50" r="D12" t="s">
+      <c s="237" r="C12" t="n"/>
+      <c s="239" r="D12" t="s">
         <v>14</v>
       </c>
       <c s="179" r="E12" t="n">
         <v>3</v>
       </c>
-      <c s="236" r="F12" t="n"/>
+      <c s="237" r="F12" t="n"/>
       <c s="179" r="G12" t="n">
         <v>20</v>
       </c>
-      <c s="236" r="H12" t="n"/>
+      <c s="237" r="H12" t="n"/>
       <c s="14" r="I12" t="n">
         <v>4</v>
       </c>
@@ -2803,18 +2903,18 @@
       <c s="174" r="B13" t="s">
         <v>16</v>
       </c>
-      <c s="236" r="C13" t="n"/>
-      <c s="50" r="D13" t="s">
+      <c s="237" r="C13" t="n"/>
+      <c s="239" r="D13" t="s">
         <v>17</v>
       </c>
       <c s="179" r="E13" t="n">
         <v>310</v>
       </c>
-      <c s="236" r="F13" t="n"/>
+      <c s="237" r="F13" t="n"/>
       <c s="179" r="G13" t="s">
         <v>18</v>
       </c>
-      <c s="236" r="H13" t="n"/>
+      <c s="237" r="H13" t="n"/>
       <c s="14" r="I13" t="n">
         <v>210</v>
       </c>
@@ -2823,18 +2923,18 @@
       <c s="174" r="B14" t="s">
         <v>19</v>
       </c>
-      <c s="236" r="C14" t="n"/>
-      <c s="50" r="D14" t="s">
+      <c s="237" r="C14" t="n"/>
+      <c s="239" r="D14" t="s">
         <v>20</v>
       </c>
       <c s="179" r="E14" t="n">
         <v>34</v>
       </c>
-      <c s="236" r="F14" t="n"/>
+      <c s="237" r="F14" t="n"/>
       <c s="179" r="G14" t="n">
         <v>150</v>
       </c>
-      <c s="236" r="H14" t="n"/>
+      <c s="237" r="H14" t="n"/>
       <c s="14" r="I14" t="n">
         <v>30</v>
       </c>
@@ -2843,18 +2943,18 @@
       <c s="174" r="B15" t="s">
         <v>21</v>
       </c>
-      <c s="236" r="C15" t="n"/>
-      <c s="50" r="D15" t="s">
+      <c s="237" r="C15" t="n"/>
+      <c s="239" r="D15" t="s">
         <v>22</v>
       </c>
       <c s="179" r="E15" t="n">
         <v>400</v>
       </c>
-      <c s="236" r="F15" t="n"/>
+      <c s="237" r="F15" t="n"/>
       <c s="179" r="G15" t="s">
         <v>18</v>
       </c>
-      <c s="236" r="H15" t="n"/>
+      <c s="237" r="H15" t="n"/>
       <c s="14" r="I15" t="n">
         <v>150</v>
       </c>
@@ -2863,18 +2963,18 @@
       <c s="174" r="B16" t="s">
         <v>23</v>
       </c>
-      <c s="236" r="C16" t="n"/>
-      <c s="50" r="D16" t="s">
+      <c s="237" r="C16" t="n"/>
+      <c s="239" r="D16" t="s">
         <v>24</v>
       </c>
       <c s="179" r="E16" t="n">
         <v>150</v>
       </c>
-      <c s="236" r="F16" t="n"/>
+      <c s="237" r="F16" t="n"/>
       <c s="179" r="G16" t="n">
         <v>500</v>
       </c>
-      <c s="236" r="H16" t="n"/>
+      <c s="237" r="H16" t="n"/>
       <c s="14" r="I16" t="n">
         <v>100</v>
       </c>
@@ -2883,18 +2983,18 @@
       <c s="174" r="B17" t="s">
         <v>25</v>
       </c>
-      <c s="236" r="C17" t="n"/>
-      <c s="50" r="D17" t="s">
+      <c s="237" r="C17" t="n"/>
+      <c s="239" r="D17" t="s">
         <v>14</v>
       </c>
       <c s="179" r="E17" t="n">
         <v>0.08</v>
       </c>
-      <c s="236" r="F17" t="n"/>
+      <c s="237" r="F17" t="n"/>
       <c s="179" r="G17" t="n">
         <v>5</v>
       </c>
-      <c s="236" r="H17" t="n"/>
+      <c s="237" r="H17" t="n"/>
       <c s="14" r="I17" t="n">
         <v>1</v>
       </c>
@@ -2903,18 +3003,18 @@
       <c s="174" r="B18" t="s">
         <v>26</v>
       </c>
-      <c s="236" r="C18" t="n"/>
-      <c s="50" r="D18" t="s">
+      <c s="237" r="C18" t="n"/>
+      <c s="239" r="D18" t="s">
         <v>27</v>
       </c>
       <c s="179" r="E18" t="n">
         <v>5</v>
       </c>
-      <c s="236" r="F18" t="n"/>
+      <c s="237" r="F18" t="n"/>
       <c s="179" r="G18" t="n">
         <v>20</v>
       </c>
-      <c s="236" r="H18" t="n"/>
+      <c s="237" r="H18" t="n"/>
       <c s="14" r="I18" t="n">
         <v>4</v>
       </c>
@@ -2923,18 +3023,18 @@
       <c s="174" r="B19" t="s">
         <v>28</v>
       </c>
-      <c s="236" r="C19" t="n"/>
-      <c s="50" r="D19" t="s">
+      <c s="237" r="C19" t="n"/>
+      <c s="239" r="D19" t="s">
         <v>29</v>
       </c>
       <c s="179" r="E19" t="n">
         <v>62</v>
       </c>
-      <c s="236" r="F19" t="n"/>
+      <c s="237" r="F19" t="n"/>
       <c s="179" r="G19" t="n">
         <v>180</v>
       </c>
-      <c s="236" r="H19" t="n"/>
+      <c s="237" r="H19" t="n"/>
       <c s="14" r="I19" t="n">
         <v>36</v>
       </c>
@@ -2943,18 +3043,18 @@
       <c s="174" r="B20" t="s">
         <v>30</v>
       </c>
-      <c s="236" r="C20" t="n"/>
-      <c s="50" r="D20" t="s">
+      <c s="237" r="C20" t="n"/>
+      <c s="239" r="D20" t="s">
         <v>14</v>
       </c>
       <c s="179" r="E20" t="n">
         <v>2</v>
       </c>
-      <c s="236" r="F20" t="n"/>
+      <c s="237" r="F20" t="n"/>
       <c s="179" r="G20" t="n">
         <v>14</v>
       </c>
-      <c s="236" r="H20" t="n"/>
+      <c s="237" r="H20" t="n"/>
       <c s="14" r="I20" t="n">
         <v>2.8</v>
       </c>
@@ -2963,18 +3063,18 @@
       <c s="181" r="B21" t="s">
         <v>31</v>
       </c>
-      <c s="237" r="C21" t="n"/>
-      <c s="51" r="D21" t="s">
+      <c s="240" r="C21" t="n"/>
+      <c s="241" r="D21" t="s">
         <v>32</v>
       </c>
       <c s="183" r="E21" t="n">
         <v>700</v>
       </c>
-      <c s="237" r="F21" t="n"/>
+      <c s="240" r="F21" t="n"/>
       <c s="183" r="G21" t="n">
         <v>1850</v>
       </c>
-      <c s="237" r="H21" t="n"/>
+      <c s="240" r="H21" t="n"/>
       <c s="15" r="I21" t="n">
         <v>370</v>
       </c>
@@ -2985,85 +3085,88 @@
         <v>33</v>
       </c>
       <c s="3" r="C22" t="n"/>
-      <c s="8" r="D22" t="n"/>
+      <c s="220" r="D22" t="n"/>
       <c s="9" r="E22" t="n"/>
     </row>
     <row r="23" spans="1:9">
       <c s="2" r="A23" t="n"/>
       <c s="3" r="B23" t="n"/>
       <c s="4" r="C23" t="n"/>
-      <c s="5" r="D23" t="n"/>
+      <c s="220" r="D23" t="n"/>
       <c s="6" r="E23" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="24" ht="16.5" spans="1:9">
       <c s="165" r="A24" t="s">
         <v>34</v>
       </c>
+      <c s="220" r="D24" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="25" ht="16.5" spans="1:9">
-      <c s="238" r="B25" t="s">
+      <c s="242" r="B25" t="s">
         <v>35</v>
       </c>
-      <c s="239" r="C25" t="n"/>
-      <c s="240" r="D25" t="s">
+      <c s="243" r="C25" t="n"/>
+      <c s="223" r="D25" t="s">
         <v>5</v>
       </c>
-      <c s="241" r="E25" t="n"/>
-      <c s="221" r="F25" t="n"/>
-      <c s="221" r="G25" t="n"/>
-      <c s="221" r="H25" t="n"/>
-      <c s="231" r="I25" t="n"/>
+      <c s="244" r="E25" t="n"/>
+      <c s="222" r="F25" t="n"/>
+      <c s="222" r="G25" t="n"/>
+      <c s="222" r="H25" t="n"/>
+      <c s="232" r="I25" t="n"/>
     </row>
     <row r="26" spans="1:9">
       <c s="170" r="B26" t="s">
         <v>36</v>
       </c>
-      <c s="242" r="C26" t="n"/>
-      <c s="49" r="D26" t="s">
+      <c s="245" r="C26" t="n"/>
+      <c s="238" r="D26" t="s">
         <v>14</v>
       </c>
       <c s="172" r="E26" t="n"/>
-      <c s="242" r="F26" t="n"/>
-      <c s="242" r="G26" t="n"/>
-      <c s="242" r="H26" t="n"/>
-      <c s="243" r="I26" t="n"/>
+      <c s="245" r="F26" t="n"/>
+      <c s="245" r="G26" t="n"/>
+      <c s="245" r="H26" t="n"/>
+      <c s="246" r="I26" t="n"/>
     </row>
     <row customHeight="1" r="27" ht="15" spans="1:9">
       <c s="174" r="B27" t="s">
         <v>37</v>
       </c>
-      <c s="236" r="C27" t="n"/>
-      <c s="50" r="D27" t="s">
+      <c s="237" r="C27" t="n"/>
+      <c s="239" r="D27" t="s">
         <v>14</v>
       </c>
       <c s="176" r="E27" t="n"/>
-      <c s="236" r="F27" t="n"/>
-      <c s="236" r="G27" t="n"/>
-      <c s="236" r="H27" t="n"/>
-      <c s="244" r="I27" t="n"/>
+      <c s="237" r="F27" t="n"/>
+      <c s="237" r="G27" t="n"/>
+      <c s="237" r="H27" t="n"/>
+      <c s="247" r="I27" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="28" ht="15" spans="1:9">
       <c s="154" r="B28" t="s">
         <v>38</v>
       </c>
-      <c s="237" r="C28" t="n"/>
-      <c s="51" r="D28" t="s">
+      <c s="240" r="C28" t="n"/>
+      <c s="241" r="D28" t="s">
         <v>39</v>
       </c>
       <c s="156" r="E28" t="n"/>
-      <c s="237" r="F28" t="n"/>
-      <c s="237" r="G28" t="n"/>
-      <c s="237" r="H28" t="n"/>
-      <c s="245" r="I28" t="n"/>
-    </row>
-    <row customHeight="1" r="29" ht="15" spans="1:9"/>
+      <c s="240" r="F28" t="n"/>
+      <c s="240" r="G28" t="n"/>
+      <c s="240" r="H28" t="n"/>
+      <c s="248" r="I28" t="n"/>
+    </row>
+    <row customHeight="1" r="29" ht="15" spans="1:9">
+      <c s="220" r="D29" t="n"/>
+    </row>
     <row customHeight="1" thickBot="1" r="30" ht="16.5" spans="1:9">
       <c s="39" r="A30" t="s">
         <v>40</v>
       </c>
       <c s="20" r="B30" t="n"/>
       <c s="39" r="C30" t="n"/>
-      <c s="20" r="D30" t="n"/>
+      <c s="220" r="D30" t="n"/>
       <c s="20" r="E30" t="n"/>
       <c s="20" r="F30" t="n"/>
       <c s="20" r="G30" t="n"/>
@@ -3074,25 +3177,25 @@
       <c s="158" r="B31" t="s">
         <v>41</v>
       </c>
-      <c s="221" r="C31" t="n"/>
-      <c s="159" r="D31" t="s">
+      <c s="222" r="C31" t="n"/>
+      <c s="249" r="D31" t="s">
         <v>5</v>
       </c>
       <c s="159" r="E31" t="s">
         <v>42</v>
       </c>
-      <c s="221" r="F31" t="n"/>
-      <c s="221" r="G31" t="n"/>
+      <c s="222" r="F31" t="n"/>
+      <c s="222" r="G31" t="n"/>
       <c s="159" r="H31" t="s">
         <v>7</v>
       </c>
-      <c s="231" r="I31" t="n"/>
+      <c s="232" r="I31" t="n"/>
     </row>
     <row customHeight="1" r="32" ht="15" spans="1:9">
       <c s="161" r="B32" t="s">
         <v>43</v>
       </c>
-      <c s="22" r="D32" t="s">
+      <c s="250" r="D32" t="s">
         <v>44</v>
       </c>
       <c s="163" r="E32" t="s">
@@ -3101,46 +3204,48 @@
       <c s="163" r="H32" t="s">
         <v>45</v>
       </c>
-      <c s="246" r="I32" t="n"/>
+      <c s="251" r="I32" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="33" ht="15" spans="1:9">
       <c s="140" r="B33" t="s">
         <v>46</v>
       </c>
-      <c s="237" r="C33" t="n"/>
-      <c s="23" r="D33" t="s">
+      <c s="240" r="C33" t="n"/>
+      <c s="252" r="D33" t="s">
         <v>47</v>
       </c>
       <c s="142" r="E33" t="s">
         <v>48</v>
       </c>
-      <c s="237" r="F33" t="n"/>
-      <c s="237" r="G33" t="n"/>
+      <c s="240" r="F33" t="n"/>
+      <c s="240" r="G33" t="n"/>
       <c s="142" r="H33" t="s">
         <v>49</v>
       </c>
-      <c s="245" r="I33" t="n"/>
+      <c s="248" r="I33" t="n"/>
     </row>
     <row customFormat="1" customHeight="1" s="24" r="34" spans="1:9" ht="15">
       <c s="3" r="B34" t="s">
         <v>33</v>
       </c>
       <c s="3" r="C34" t="n"/>
-      <c s="8" r="D34" t="n"/>
+      <c s="220" r="D34" t="n"/>
       <c s="9" r="E34" t="n"/>
       <c s="25" r="F34" t="n"/>
       <c s="25" r="G34" t="n"/>
       <c s="25" r="H34" t="n"/>
       <c s="25" r="I34" t="n"/>
     </row>
-    <row customHeight="1" r="35" ht="15" spans="1:9"/>
+    <row customHeight="1" r="35" ht="15" spans="1:9">
+      <c s="220" r="D35" t="n"/>
+    </row>
     <row customHeight="1" thickBot="1" r="36" ht="16.5" spans="1:9">
       <c s="39" r="A36" t="s">
         <v>50</v>
       </c>
       <c s="20" r="B36" t="n"/>
       <c s="39" r="C36" t="n"/>
-      <c s="20" r="D36" t="n"/>
+      <c s="220" r="D36" t="n"/>
       <c s="20" r="E36" t="n"/>
       <c s="20" r="F36" t="n"/>
       <c s="20" r="G36" t="n"/>
@@ -3152,7 +3257,7 @@
         <v>51</v>
       </c>
       <c s="41" r="C37" t="n"/>
-      <c s="34" r="D37" t="s">
+      <c s="249" r="D37" t="s">
         <v>5</v>
       </c>
       <c s="44" r="E37" t="s">
@@ -3167,71 +3272,85 @@
       <c s="90" r="B38" t="s">
         <v>53</v>
       </c>
-      <c s="247" r="C38" t="n"/>
-      <c s="64" r="D38" t="s">
+      <c s="253" r="C38" t="n"/>
+      <c s="254" r="D38" t="s">
         <v>54</v>
       </c>
       <c s="45" r="E38" t="s">
         <v>55</v>
       </c>
       <c s="145" r="F38" t="n"/>
-      <c s="247" r="G38" t="n"/>
-      <c s="247" r="H38" t="n"/>
-      <c s="248" r="I38" t="n"/>
+      <c s="253" r="G38" t="n"/>
+      <c s="253" r="H38" t="n"/>
+      <c s="255" r="I38" t="n"/>
     </row>
     <row customHeight="1" r="39" ht="15" spans="1:9">
       <c s="75" r="B39" t="s">
         <v>56</v>
       </c>
-      <c s="247" r="C39" t="n"/>
-      <c s="53" r="D39" t="s">
+      <c s="253" r="C39" t="n"/>
+      <c s="239" r="D39" t="s">
         <v>57</v>
       </c>
       <c s="46" r="E39" t="s">
         <v>58</v>
       </c>
       <c s="148" r="F39" t="n"/>
-      <c s="247" r="G39" t="n"/>
-      <c s="247" r="H39" t="n"/>
-      <c s="248" r="I39" t="n"/>
+      <c s="253" r="G39" t="n"/>
+      <c s="253" r="H39" t="n"/>
+      <c s="255" r="I39" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="40" ht="15" spans="1:9">
       <c s="78" r="B40" t="s">
         <v>59</v>
       </c>
-      <c s="237" r="C40" t="n"/>
-      <c s="54" r="D40" t="s">
+      <c s="240" r="C40" t="n"/>
+      <c s="241" r="D40" t="s">
         <v>60</v>
       </c>
       <c s="47" r="E40" t="s">
         <v>61</v>
       </c>
       <c s="151" r="F40" t="n"/>
-      <c s="237" r="G40" t="n"/>
-      <c s="237" r="H40" t="n"/>
-      <c s="245" r="I40" t="n"/>
-    </row>
-    <row customHeight="1" r="41" ht="15" spans="1:9"/>
-    <row customHeight="1" r="42" ht="15" spans="1:9"/>
-    <row customHeight="1" r="43" ht="15" spans="1:9"/>
-    <row customHeight="1" r="44" ht="15" spans="1:9"/>
-    <row customHeight="1" r="45" ht="15" spans="1:9"/>
-    <row customHeight="1" r="46" ht="15" spans="1:9"/>
+      <c s="240" r="G40" t="n"/>
+      <c s="240" r="H40" t="n"/>
+      <c s="248" r="I40" t="n"/>
+    </row>
+    <row customHeight="1" r="41" ht="15" spans="1:9">
+      <c s="220" r="D41" t="n"/>
+    </row>
+    <row customHeight="1" r="42" ht="15" spans="1:9">
+      <c s="220" r="D42" t="n"/>
+    </row>
+    <row customHeight="1" r="43" ht="15" spans="1:9">
+      <c s="220" r="D43" t="n"/>
+    </row>
+    <row customHeight="1" r="44" ht="15" spans="1:9">
+      <c s="220" r="D44" t="n"/>
+    </row>
+    <row customHeight="1" r="45" ht="15" spans="1:9">
+      <c s="220" r="D45" t="n"/>
+    </row>
+    <row customHeight="1" r="46" ht="15" spans="1:9">
+      <c s="220" r="D46" t="n"/>
+    </row>
     <row customHeight="1" r="47" ht="15" spans="1:9">
       <c s="144" r="A47" t="s">
         <v>62</v>
       </c>
+      <c s="220" r="D47" t="n"/>
     </row>
     <row customHeight="1" r="48" ht="30.75" spans="1:9">
       <c s="144" r="A48" t="s">
         <v>63</v>
       </c>
+      <c s="220" r="D48" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="49" ht="15" spans="1:9">
       <c s="48" r="A49" t="n"/>
       <c s="48" r="B49" t="n"/>
       <c s="48" r="C49" t="n"/>
-      <c s="27" r="D49" t="n"/>
+      <c s="220" r="D49" t="n"/>
       <c s="6" r="E49" t="n"/>
       <c s="6" r="F49" t="n"/>
       <c s="6" r="G49" t="n"/>
@@ -3242,70 +3361,72 @@
       <c s="122" r="A50" t="s">
         <v>64</v>
       </c>
-      <c s="221" r="B50" t="n"/>
-      <c s="221" r="C50" t="n"/>
-      <c s="123" r="D50" t="s">
+      <c s="222" r="B50" t="n"/>
+      <c s="222" r="C50" t="n"/>
+      <c s="249" r="D50" t="s">
         <v>5</v>
       </c>
       <c s="128" r="E50" t="n"/>
-      <c s="221" r="F50" t="n"/>
-      <c s="221" r="G50" t="n"/>
-      <c s="221" r="H50" t="n"/>
-      <c s="231" r="I50" t="n"/>
+      <c s="222" r="F50" t="n"/>
+      <c s="222" r="G50" t="n"/>
+      <c s="222" r="H50" t="n"/>
+      <c s="232" r="I50" t="n"/>
     </row>
     <row customHeight="1" r="51" ht="15" spans="1:9">
       <c s="124" r="A51" t="s">
         <v>65</v>
       </c>
-      <c s="247" r="B51" t="n"/>
-      <c s="247" r="C51" t="n"/>
-      <c s="52" r="D51" t="s">
+      <c s="253" r="B51" t="n"/>
+      <c s="253" r="C51" t="n"/>
+      <c s="254" r="D51" t="s">
         <v>66</v>
       </c>
       <c s="137" r="E51" t="n"/>
-      <c s="247" r="F51" t="n"/>
-      <c s="247" r="G51" t="n"/>
-      <c s="247" r="H51" t="n"/>
-      <c s="248" r="I51" t="n"/>
+      <c s="253" r="F51" t="n"/>
+      <c s="253" r="G51" t="n"/>
+      <c s="253" r="H51" t="n"/>
+      <c s="255" r="I51" t="n"/>
     </row>
     <row customHeight="1" r="52" ht="15" spans="1:9">
       <c s="120" r="A52" t="s">
         <v>67</v>
       </c>
-      <c s="247" r="B52" t="n"/>
-      <c s="247" r="C52" t="n"/>
-      <c s="65" r="D52" t="n">
+      <c s="253" r="B52" t="n"/>
+      <c s="253" r="C52" t="n"/>
+      <c s="239" r="D52" t="n">
         <v>86.45279999999998</v>
       </c>
       <c s="134" r="E52" t="n"/>
-      <c s="247" r="F52" t="n"/>
-      <c s="247" r="G52" t="n"/>
-      <c s="247" r="H52" t="n"/>
-      <c s="248" r="I52" t="n"/>
+      <c s="253" r="F52" t="n"/>
+      <c s="253" r="G52" t="n"/>
+      <c s="253" r="H52" t="n"/>
+      <c s="255" r="I52" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="53" ht="15" spans="1:9">
       <c s="126" r="A53" t="s">
         <v>68</v>
       </c>
-      <c s="249" r="B53" t="n"/>
-      <c s="249" r="C53" t="n"/>
-      <c s="51" r="D53" t="n">
+      <c s="256" r="B53" t="n"/>
+      <c s="256" r="C53" t="n"/>
+      <c s="241" r="D53" t="n">
         <v>176.4288</v>
       </c>
       <c s="131" r="E53" t="n"/>
-      <c s="249" r="F53" t="n"/>
-      <c s="249" r="G53" t="n"/>
-      <c s="249" r="H53" t="n"/>
-      <c s="250" r="I53" t="n"/>
-    </row>
-    <row customHeight="1" thickBot="1" r="54" ht="15" spans="1:9"/>
+      <c s="256" r="F53" t="n"/>
+      <c s="256" r="G53" t="n"/>
+      <c s="256" r="H53" t="n"/>
+      <c s="257" r="I53" t="n"/>
+    </row>
+    <row customHeight="1" thickBot="1" r="54" ht="15" spans="1:9">
+      <c s="220" r="D54" t="n"/>
+    </row>
     <row customHeight="1" r="55" ht="15" spans="1:9">
       <c s="107" r="A55" t="s">
         <v>69</v>
       </c>
-      <c s="251" r="B55" t="n"/>
-      <c s="251" r="C55" t="n"/>
-      <c s="111" r="D55" t="s">
+      <c s="258" r="B55" t="n"/>
+      <c s="258" r="C55" t="n"/>
+      <c s="259" r="D55" t="s">
         <v>5</v>
       </c>
       <c s="113" r="E55" t="s">
@@ -3314,25 +3435,26 @@
       <c s="115" r="F55" t="s">
         <v>71</v>
       </c>
-      <c s="251" r="G55" t="n"/>
-      <c s="251" r="H55" t="n"/>
-      <c s="252" r="I55" t="n"/>
+      <c s="258" r="G55" t="n"/>
+      <c s="258" r="H55" t="n"/>
+      <c s="260" r="I55" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="56" ht="15" spans="1:9">
-      <c s="249" r="B56" t="n"/>
-      <c s="249" r="C56" t="n"/>
-      <c s="249" r="D56" t="n"/>
-      <c s="249" r="E56" t="n"/>
-      <c s="36" r="F56" t="s">
+      <c s="261" r="A56" t="n"/>
+      <c s="256" r="B56" t="n"/>
+      <c s="256" r="C56" t="n"/>
+      <c s="262" r="D56" t="n"/>
+      <c s="256" r="E56" t="n"/>
+      <c s="263" r="F56" t="s">
         <v>72</v>
       </c>
-      <c s="36" r="G56" t="s">
+      <c s="263" r="G56" t="s">
         <v>73</v>
       </c>
-      <c s="36" r="H56" t="s">
+      <c s="263" r="H56" t="s">
         <v>74</v>
       </c>
-      <c s="37" r="I56" t="s">
+      <c s="264" r="I56" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3340,96 +3462,100 @@
       <c s="214" r="A57" t="s">
         <v>76</v>
       </c>
+      <c s="220" r="D57" t="n"/>
+      <c s="251" r="I57" t="n"/>
     </row>
     <row customHeight="1" r="58" ht="15" spans="1:9">
       <c s="105" r="A58" t="s">
         <v>77</v>
       </c>
-      <c s="251" r="B58" t="n"/>
-      <c s="251" r="C58" t="n"/>
-      <c s="66" r="D58" t="s">
+      <c s="258" r="B58" t="n"/>
+      <c s="258" r="C58" t="n"/>
+      <c s="265" r="D58" t="s">
         <v>78</v>
       </c>
       <c s="28" r="E58" t="s">
         <v>61</v>
       </c>
       <c s="117" r="F58" t="n"/>
-      <c s="251" r="G58" t="n"/>
-      <c s="251" r="H58" t="n"/>
-      <c s="252" r="I58" t="n"/>
+      <c s="258" r="G58" t="n"/>
+      <c s="258" r="H58" t="n"/>
+      <c s="260" r="I58" t="n"/>
     </row>
     <row customHeight="1" r="59" ht="15" spans="1:9">
       <c s="95" r="A59" t="s">
         <v>79</v>
       </c>
-      <c s="236" r="B59" t="n"/>
-      <c s="236" r="C59" t="n"/>
-      <c s="67" r="D59" t="s">
+      <c s="237" r="B59" t="n"/>
+      <c s="237" r="C59" t="n"/>
+      <c s="266" r="D59" t="s">
         <v>80</v>
       </c>
       <c s="29" r="E59" t="n"/>
       <c s="99" r="F59" t="n"/>
-      <c s="236" r="G59" t="n"/>
-      <c s="236" r="H59" t="n"/>
-      <c s="244" r="I59" t="n"/>
+      <c s="237" r="G59" t="n"/>
+      <c s="237" r="H59" t="n"/>
+      <c s="247" r="I59" t="n"/>
     </row>
     <row customHeight="1" r="60" ht="15" spans="1:9">
       <c s="95" r="A60" t="s">
         <v>81</v>
       </c>
-      <c s="236" r="B60" t="n"/>
-      <c s="236" r="C60" t="n"/>
-      <c s="67" r="D60" t="s">
+      <c s="237" r="B60" t="n"/>
+      <c s="237" r="C60" t="n"/>
+      <c s="266" r="D60" t="s">
         <v>82</v>
       </c>
       <c s="29" r="E60" t="n"/>
       <c s="99" r="F60" t="n"/>
-      <c s="236" r="G60" t="n"/>
-      <c s="236" r="H60" t="n"/>
-      <c s="244" r="I60" t="n"/>
+      <c s="237" r="G60" t="n"/>
+      <c s="237" r="H60" t="n"/>
+      <c s="247" r="I60" t="n"/>
     </row>
     <row customHeight="1" r="61" ht="15" spans="1:9">
       <c s="97" r="A61" t="s">
         <v>83</v>
       </c>
-      <c s="236" r="B61" t="n"/>
-      <c s="236" r="C61" t="n"/>
-      <c s="67" r="D61" t="s">
+      <c s="237" r="B61" t="n"/>
+      <c s="237" r="C61" t="n"/>
+      <c s="266" r="D61" t="s">
         <v>84</v>
       </c>
       <c s="29" r="E61" t="n"/>
       <c s="99" r="F61" t="n"/>
-      <c s="236" r="G61" t="n"/>
-      <c s="236" r="H61" t="n"/>
-      <c s="244" r="I61" t="n"/>
+      <c s="237" r="G61" t="n"/>
+      <c s="237" r="H61" t="n"/>
+      <c s="247" r="I61" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="62" ht="15" spans="1:9">
       <c s="93" r="A62" t="s">
         <v>85</v>
       </c>
-      <c s="249" r="B62" t="n"/>
-      <c s="249" r="C62" t="n"/>
-      <c s="68" r="D62" t="s"/>
+      <c s="256" r="B62" t="n"/>
+      <c s="256" r="C62" t="n"/>
+      <c s="267" r="D62" t="s"/>
       <c s="30" r="E62" t="s">
         <v>86</v>
       </c>
       <c s="102" r="F62" t="n"/>
-      <c s="249" r="G62" t="n"/>
-      <c s="249" r="H62" t="n"/>
-      <c s="250" r="I62" t="n"/>
+      <c s="256" r="G62" t="n"/>
+      <c s="256" r="H62" t="n"/>
+      <c s="257" r="I62" t="n"/>
     </row>
     <row customHeight="1" thickBot="1" r="63" ht="15" spans="1:9">
       <c s="217" r="A63" t="s">
         <v>87</v>
       </c>
+      <c s="220" r="D63" t="n"/>
+      <c s="251" r="I63" t="n"/>
     </row>
     <row customHeight="1" r="64" ht="15" spans="1:9">
       <c s="90" r="A64" t="s">
         <v>88</v>
       </c>
-      <c s="251" r="B64" t="n"/>
-      <c s="251" r="C64" t="n"/>
-      <c s="69" r="D64" t="n">
+      <c s="258" r="B64" t="n"/>
+      <c s="258" r="C64" t="n"/>
+      <c s="265" r="D64" t="n">
         <v>0.2</v>
       </c>
       <c s="31" r="E64" t="s">
@@ -3456,9 +3582,9 @@
       <c s="75" r="A65" t="s">
         <v>89</v>
       </c>
-      <c s="236" r="B65" t="n"/>
-      <c s="236" r="C65" t="n"/>
-      <c s="70" r="D65" t="s">
+      <c s="237" r="B65" t="n"/>
+      <c s="237" r="C65" t="n"/>
+      <c s="266" r="D65" t="s">
         <v>66</v>
       </c>
       <c s="32" r="E65" t="s">
@@ -3485,9 +3611,9 @@
       <c s="75" r="A66" t="s">
         <v>91</v>
       </c>
-      <c s="236" r="B66" t="n"/>
-      <c s="236" r="C66" t="n"/>
-      <c s="70" r="D66" t="n">
+      <c s="237" r="B66" t="n"/>
+      <c s="237" r="C66" t="n"/>
+      <c s="266" r="D66" t="n">
         <v>1.14048</v>
       </c>
       <c s="32" r="E66" t="s">
@@ -3514,9 +3640,9 @@
       <c s="87" r="A67" t="s">
         <v>92</v>
       </c>
-      <c s="236" r="B67" t="n"/>
-      <c s="236" r="C67" t="n"/>
-      <c s="70" r="D67" t="n">
+      <c s="237" r="B67" t="n"/>
+      <c s="237" r="C67" t="n"/>
+      <c s="266" r="D67" t="n">
         <v>0.159384</v>
       </c>
       <c s="32" r="E67" t="s">
@@ -3543,9 +3669,9 @@
       <c s="81" r="A68" t="s">
         <v>93</v>
       </c>
-      <c s="236" r="B68" t="n"/>
-      <c s="236" r="C68" t="n"/>
-      <c s="70" r="D68" t="n">
+      <c s="237" r="B68" t="n"/>
+      <c s="237" r="C68" t="n"/>
+      <c s="266" r="D68" t="n">
         <v>0.155364</v>
       </c>
       <c s="32" r="E68" t="s">
@@ -3572,9 +3698,9 @@
       <c s="84" r="A69" t="s">
         <v>94</v>
       </c>
-      <c s="236" r="B69" t="n"/>
-      <c s="236" r="C69" t="n"/>
-      <c s="70" r="D69" t="n">
+      <c s="237" r="B69" t="n"/>
+      <c s="237" r="C69" t="n"/>
+      <c s="266" r="D69" t="n">
         <v>0.0122184</v>
       </c>
       <c s="32" r="E69" t="s">
@@ -3601,9 +3727,9 @@
       <c s="72" r="A70" t="s">
         <v>95</v>
       </c>
-      <c s="236" r="B70" t="n"/>
-      <c s="236" r="C70" t="n"/>
-      <c s="70" r="D70" t="n">
+      <c s="237" r="B70" t="n"/>
+      <c s="237" r="C70" t="n"/>
+      <c s="266" r="D70" t="n">
         <v>0.1128</v>
       </c>
       <c s="29" r="E70" t="s">
@@ -3630,9 +3756,9 @@
       <c s="75" r="A71" t="s">
         <v>96</v>
       </c>
-      <c s="236" r="B71" t="n"/>
-      <c s="236" r="C71" t="n"/>
-      <c s="70" r="D71" t="n">
+      <c s="237" r="B71" t="n"/>
+      <c s="237" r="C71" t="n"/>
+      <c s="266" r="D71" t="n">
         <v>0.00282144</v>
       </c>
       <c s="32" r="E71" t="s">
@@ -3659,9 +3785,9 @@
       <c s="75" r="A72" t="s">
         <v>97</v>
       </c>
-      <c s="236" r="B72" t="n"/>
-      <c s="236" r="C72" t="n"/>
-      <c s="70" r="D72" t="n">
+      <c s="237" r="B72" t="n"/>
+      <c s="237" r="C72" t="n"/>
+      <c s="266" r="D72" t="n">
         <v>0.0192</v>
       </c>
       <c s="32" r="E72" t="s">
@@ -3688,9 +3814,9 @@
       <c s="75" r="A73" t="s">
         <v>98</v>
       </c>
-      <c s="236" r="B73" t="n"/>
-      <c s="236" r="C73" t="n"/>
-      <c s="70" r="D73" t="n">
+      <c s="237" r="B73" t="n"/>
+      <c s="237" r="C73" t="n"/>
+      <c s="266" r="D73" t="n">
         <v>0.04085376</v>
       </c>
       <c s="32" r="E73" t="s">
@@ -3717,9 +3843,9 @@
       <c s="75" r="A74" t="s">
         <v>99</v>
       </c>
-      <c s="236" r="B74" t="n"/>
-      <c s="236" r="C74" t="n"/>
-      <c s="70" r="D74" t="n">
+      <c s="237" r="B74" t="n"/>
+      <c s="237" r="C74" t="n"/>
+      <c s="266" r="D74" t="n">
         <v>0.28944</v>
       </c>
       <c s="32" r="E74" t="s">
@@ -3746,9 +3872,9 @@
       <c s="75" r="A75" t="s">
         <v>100</v>
       </c>
-      <c s="236" r="B75" t="n"/>
-      <c s="236" r="C75" t="n"/>
-      <c s="70" r="D75" t="n">
+      <c s="237" r="B75" t="n"/>
+      <c s="237" r="C75" t="n"/>
+      <c s="266" r="D75" t="n">
         <v>9.6</v>
       </c>
       <c s="32" r="E75" t="s">
@@ -3775,9 +3901,9 @@
       <c s="75" r="A76" t="s">
         <v>101</v>
       </c>
-      <c s="236" r="B76" t="n"/>
-      <c s="236" r="C76" t="n"/>
-      <c s="70" r="D76" t="n">
+      <c s="237" r="B76" t="n"/>
+      <c s="237" r="C76" t="n"/>
+      <c s="266" r="D76" t="n">
         <v>320.88</v>
       </c>
       <c s="32" r="E76" t="s">
@@ -3804,9 +3930,9 @@
       <c s="72" r="A77" t="s">
         <v>102</v>
       </c>
-      <c s="236" r="B77" t="n"/>
-      <c s="236" r="C77" t="n"/>
-      <c s="70" r="D77" t="n">
+      <c s="237" r="B77" t="n"/>
+      <c s="237" r="C77" t="n"/>
+      <c s="266" r="D77" t="n">
         <v>1.1472</v>
       </c>
       <c s="29" r="E77" t="s">
@@ -3833,9 +3959,9 @@
       <c s="72" r="A78" t="s">
         <v>103</v>
       </c>
-      <c s="236" r="B78" t="n"/>
-      <c s="236" r="C78" t="n"/>
-      <c s="70" r="D78" t="n">
+      <c s="237" r="B78" t="n"/>
+      <c s="237" r="C78" t="n"/>
+      <c s="266" r="D78" t="n">
         <v>1802.88</v>
       </c>
       <c s="29" r="E78" t="s">
@@ -3862,9 +3988,9 @@
       <c s="72" r="A79" t="s">
         <v>104</v>
       </c>
-      <c s="236" r="B79" t="n"/>
-      <c s="236" r="C79" t="n"/>
-      <c s="70" r="D79" t="n">
+      <c s="237" r="B79" t="n"/>
+      <c s="237" r="C79" t="n"/>
+      <c s="266" r="D79" t="n">
         <v>3.3672</v>
       </c>
       <c s="29" r="E79" t="s">
@@ -3891,9 +4017,9 @@
       <c s="72" r="A80" t="s">
         <v>105</v>
       </c>
-      <c s="236" r="B80" t="n"/>
-      <c s="236" r="C80" t="n"/>
-      <c s="70" r="D80" t="n">
+      <c s="237" r="B80" t="n"/>
+      <c s="237" r="C80" t="n"/>
+      <c s="266" r="D80" t="n">
         <v>317.04</v>
       </c>
       <c s="29" r="E80" t="s">
@@ -3920,9 +4046,9 @@
       <c s="72" r="A81" t="s">
         <v>106</v>
       </c>
-      <c s="236" r="B81" t="n"/>
-      <c s="236" r="C81" t="n"/>
-      <c s="70" r="D81" t="n">
+      <c s="237" r="B81" t="n"/>
+      <c s="237" r="C81" t="n"/>
+      <c s="266" r="D81" t="n">
         <v>5.5464</v>
       </c>
       <c s="29" r="E81" t="s">
@@ -3949,38 +4075,34 @@
       <c s="72" r="A82" t="s">
         <v>107</v>
       </c>
-      <c s="236" r="B82" t="n"/>
-      <c s="236" r="C82" t="n"/>
-      <c s="70" r="D82" t="n">
-        <v>1.296e-05</v>
+      <c s="237" r="B82" t="n"/>
+      <c s="237" r="C82" t="n"/>
+      <c s="266" r="D82" t="s">
+        <v>14</v>
       </c>
       <c s="29" r="E82" t="s">
         <v>90</v>
       </c>
-      <c s="59" r="F82">
-        <f>D82*0.001</f>
-        <v/>
-      </c>
-      <c s="58" r="G82">
-        <f>D82*0.002</f>
-        <v/>
-      </c>
-      <c s="59" r="H82">
-        <f>D82/1000000</f>
-        <v/>
-      </c>
-      <c s="60" r="I82">
-        <f>D82/100</f>
-        <v/>
+      <c s="59" r="F82" t="s">
+        <v>108</v>
+      </c>
+      <c s="58" r="G82" t="s">
+        <v>108</v>
+      </c>
+      <c s="59" r="H82" t="s">
+        <v>108</v>
+      </c>
+      <c s="60" r="I82" t="s">
+        <v>108</v>
       </c>
     </row>
     <row customHeight="1" thickBot="1" r="83" ht="16.5" spans="1:9">
       <c s="78" r="A83" t="s">
-        <v>108</v>
-      </c>
-      <c s="249" r="B83" t="n"/>
-      <c s="249" r="C83" t="n"/>
-      <c s="71" r="D83" t="n">
+        <v>109</v>
+      </c>
+      <c s="256" r="B83" t="n"/>
+      <c s="256" r="C83" t="n"/>
+      <c s="267" r="D83" t="n">
         <v>10.9128</v>
       </c>
       <c s="33" r="E83" t="s">
@@ -4007,28 +4129,58 @@
       <c s="38" r="A84" t="n"/>
       <c s="38" r="B84" t="n"/>
       <c s="38" r="C84" t="n"/>
-      <c s="38" r="D84" t="n"/>
+      <c s="220" r="D84" t="n"/>
       <c s="38" r="E84" t="n"/>
       <c s="38" r="F84" t="n"/>
       <c s="38" r="G84" t="n"/>
       <c s="38" r="H84" t="n"/>
       <c s="38" r="I84" t="n"/>
     </row>
-    <row r="85" spans="1:9"/>
-    <row r="86" spans="1:9"/>
-    <row r="87" spans="1:9"/>
-    <row r="88" spans="1:9"/>
-    <row r="89" spans="1:9"/>
-    <row r="90" spans="1:9"/>
-    <row r="91" spans="1:9"/>
-    <row r="92" spans="1:9"/>
-    <row r="93" spans="1:9"/>
-    <row r="94" spans="1:9"/>
-    <row r="95" spans="1:9"/>
-    <row r="96" spans="1:9"/>
-    <row r="97" spans="1:9"/>
-    <row r="98" spans="1:9"/>
-    <row r="99" spans="1:9"/>
+    <row r="85" spans="1:9">
+      <c s="220" r="D85" t="n"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c s="220" r="D86" t="n"/>
+    </row>
+    <row r="87" spans="1:9">
+      <c s="220" r="D87" t="n"/>
+    </row>
+    <row r="88" spans="1:9">
+      <c s="220" r="D88" t="n"/>
+    </row>
+    <row r="89" spans="1:9">
+      <c s="220" r="D89" t="n"/>
+    </row>
+    <row r="90" spans="1:9">
+      <c s="220" r="D90" t="n"/>
+    </row>
+    <row r="91" spans="1:9">
+      <c s="220" r="D91" t="n"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c s="220" r="D92" t="n"/>
+    </row>
+    <row r="93" spans="1:9">
+      <c s="220" r="D93" t="n"/>
+    </row>
+    <row r="94" spans="1:9">
+      <c s="220" r="D94" t="n"/>
+    </row>
+    <row r="95" spans="1:9">
+      <c s="220" r="D95" t="n"/>
+    </row>
+    <row r="96" spans="1:9">
+      <c s="220" r="D96" t="n"/>
+    </row>
+    <row r="97" spans="1:9">
+      <c s="220" r="D97" t="n"/>
+    </row>
+    <row r="98" spans="1:9">
+      <c s="220" r="D98" t="n"/>
+    </row>
+    <row r="99" spans="1:9">
+      <c s="220" r="D99" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="114">
     <mergeCell ref="B12:C12"/>

</xml_diff>